<commit_message>
Brazil and Nashville updates
</commit_message>
<xml_diff>
--- a/applications/Brazil/Barretos_projections.xlsx
+++ b/applications/Brazil/Barretos_projections.xlsx
@@ -520,76 +520,76 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4">
-        <v>7321</v>
+        <v>4831</v>
       </c>
       <c r="B4">
-        <v>1203</v>
+        <v>733</v>
       </c>
       <c r="C4">
-        <v>17638</v>
+        <v>4268</v>
       </c>
       <c r="D4">
-        <v>3.327818181818182</v>
+        <v>2.195954545454544</v>
       </c>
       <c r="E4">
-        <v>0.5468636363636364</v>
+        <v>0.3333636363636364</v>
       </c>
       <c r="F4">
-        <v>8.017363636363639</v>
+        <v>1.940409090909091</v>
       </c>
       <c r="G4">
-        <v>0.6744545454545454</v>
+        <v>0.3838636363636364</v>
       </c>
       <c r="H4">
-        <v>0.1268636363636363</v>
+        <v>0.08254545454545451</v>
       </c>
       <c r="I4">
-        <v>1.298727272727272</v>
+        <v>0.291681818181818</v>
       </c>
       <c r="J4">
-        <v>0.28172</v>
+        <v>0.2013125</v>
       </c>
       <c r="K4">
-        <v>0.1520708333333333</v>
+        <v>0.1556416666666667</v>
       </c>
       <c r="L4">
-        <v>0.3387708333333334</v>
+        <v>0.1935491666666667</v>
       </c>
       <c r="M4">
-        <v>2473</v>
+        <v>3021</v>
       </c>
       <c r="N4">
-        <v>309</v>
+        <v>136</v>
       </c>
       <c r="O4">
-        <v>9922</v>
+        <v>7456</v>
       </c>
       <c r="P4">
-        <v>1.438255813953489</v>
+        <v>1.756744186046511</v>
       </c>
       <c r="Q4">
-        <v>0.18</v>
+        <v>0.07965116279069764</v>
       </c>
       <c r="R4">
-        <v>5.768720930232557</v>
+        <v>4.335174418604652</v>
       </c>
       <c r="S4">
-        <v>0.3094186046511627</v>
+        <v>0.3188372093023256</v>
       </c>
       <c r="T4">
-        <v>0.04593023255813954</v>
+        <v>0.02017441860465117</v>
       </c>
       <c r="U4">
-        <v>1.170348837209302</v>
+        <v>0.6362790697674418</v>
       </c>
       <c r="V4">
-        <v>0.2977899999999999</v>
+        <v>0.2375275</v>
       </c>
       <c r="W4">
-        <v>0.1531875</v>
+        <v>0.1572375</v>
       </c>
       <c r="X4">
-        <v>0.3993383333333334</v>
+        <v>0.2486216666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>